<commit_message>
add: Add hand light switch update: Change the behavior of the wiper switch
</commit_message>
<xml_diff>
--- a/doc/ATCFS Specifications.xlsx
+++ b/doc/ATCFS Specifications.xlsx
@@ -10,15 +10,15 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$303</definedName>
-    <definedName name="subject" localSheetId="0">Sheet1!$C$283</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$310</definedName>
+    <definedName name="subject" localSheetId="0">Sheet1!$C$285</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="489">
   <si>
     <t>Map</t>
     <phoneticPr fontId="2"/>
@@ -983,10 +983,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>ats61</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>ats8</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -1842,9 +1838,6 @@
   <si>
     <t>ATS-Pベル</t>
     <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>ワイパーON/OFFの速度調節スイッチ</t>
   </si>
   <si>
     <t>EBブザー (未実装)</t>
@@ -3126,10 +3119,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>ATC確認ボタンの解放音</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>ATC確認ボタンの押下音</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -3774,10 +3763,88 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>LCD表示切り替えスイッチ</t>
+    <t>ats206</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Needle</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ATC確認ボタンの開放音</t>
+    <rPh sb="9" eb="11">
+      <t>カイホウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LCD表示切り替えスイッチの押下音</t>
     <rPh sb="3" eb="5">
       <t>ヒョウジ</t>
     </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ats61</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ats62</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LCD表示切り替えスイッチの開放音</t>
+    <rPh sb="3" eb="5">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>手元灯表示</t>
+    <rPh sb="3" eb="5">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>電流値[A * 1000] (experimental)</t>
+    <rPh sb="0" eb="2">
+      <t>デンリュウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>7 (テンキーではない)</t>
+  </si>
+  <si>
+    <t>ATS I</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>手元灯</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ats63</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ats64</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>手元灯スイッチの押下音</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>手元灯スイッチの開放音</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ワイパーの速度調節スイッチ</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -4733,10 +4800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E303"/>
+  <dimension ref="A1:E309"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A270" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E293" sqref="E293"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A277" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A291" sqref="A291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -4752,7 +4819,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14.4" x14ac:dyDescent="0.15">
       <c r="B1" s="71" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C1" s="72"/>
       <c r="D1" s="72"/>
@@ -4770,7 +4837,7 @@
         <v>56</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -4807,7 +4874,7 @@
     <row r="7" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="12" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="14"/>
@@ -4852,16 +4919,16 @@
     <row r="12" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C12" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="E12" s="21" t="s">
         <v>315</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4873,10 +4940,10 @@
         <v>0</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4888,10 +4955,10 @@
         <v>1</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4901,10 +4968,10 @@
         <v>2</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4914,7 +4981,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E16" s="11"/>
     </row>
@@ -4925,7 +4992,7 @@
         <v>4</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E17" s="11"/>
     </row>
@@ -4936,7 +5003,7 @@
         <v>5</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E18" s="11"/>
     </row>
@@ -4947,7 +5014,7 @@
         <v>6</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E19" s="11"/>
     </row>
@@ -4958,7 +5025,7 @@
         <v>7</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E20" s="11"/>
     </row>
@@ -4969,7 +5036,7 @@
         <v>8</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E21" s="11"/>
     </row>
@@ -4980,7 +5047,7 @@
         <v>9</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E22" s="11"/>
     </row>
@@ -4991,7 +5058,7 @@
         <v>10</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E23" s="11"/>
     </row>
@@ -5002,7 +5069,7 @@
         <v>11</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E24" s="11"/>
     </row>
@@ -5013,10 +5080,10 @@
         <v>102</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5026,7 +5093,7 @@
         <v>103</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E26" s="11"/>
     </row>
@@ -5037,7 +5104,7 @@
         <v>104</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E27" s="11"/>
     </row>
@@ -5048,7 +5115,7 @@
         <v>105</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E28" s="11"/>
     </row>
@@ -5059,7 +5126,7 @@
         <v>106</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E29" s="11"/>
     </row>
@@ -5070,7 +5137,7 @@
         <v>107</v>
       </c>
       <c r="D30" s="28" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E30" s="11"/>
     </row>
@@ -5081,7 +5148,7 @@
         <v>108</v>
       </c>
       <c r="D31" s="28" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E31" s="11"/>
     </row>
@@ -5092,7 +5159,7 @@
         <v>109</v>
       </c>
       <c r="D32" s="28" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="E32" s="11"/>
     </row>
@@ -5103,7 +5170,7 @@
         <v>110</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E33" s="11"/>
     </row>
@@ -5114,7 +5181,7 @@
         <v>111</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E34" s="11"/>
     </row>
@@ -5125,7 +5192,7 @@
         <v>112</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E35" s="11"/>
     </row>
@@ -5136,7 +5203,7 @@
         <v>113</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="E36" s="14"/>
     </row>
@@ -5146,13 +5213,13 @@
         <v>50</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E37" s="33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5163,7 +5230,7 @@
       <c r="C38" s="31"/>
       <c r="D38" s="11"/>
       <c r="E38" s="33" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5181,7 +5248,7 @@
       <c r="C40" s="31"/>
       <c r="D40" s="11"/>
       <c r="E40" s="34" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5194,16 +5261,16 @@
     <row r="42" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="3"/>
       <c r="B42" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C42" s="35">
         <v>0</v>
       </c>
       <c r="D42" s="36" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5213,7 +5280,7 @@
         <v>1</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E43" s="11"/>
     </row>
@@ -5224,7 +5291,7 @@
         <v>2</v>
       </c>
       <c r="D44" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E44" s="11"/>
     </row>
@@ -5235,7 +5302,7 @@
         <v>3</v>
       </c>
       <c r="D45" s="36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E45" s="11"/>
     </row>
@@ -5246,7 +5313,7 @@
         <v>4</v>
       </c>
       <c r="D46" s="36" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E46" s="14"/>
     </row>
@@ -5289,16 +5356,16 @@
     <row r="51" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="3"/>
       <c r="B51" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C51" s="37" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5310,10 +5377,10 @@
         <v>80</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E52" s="80" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5331,7 +5398,7 @@
       <c r="C54" s="31"/>
       <c r="D54" s="11"/>
       <c r="E54" s="79" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5354,7 +5421,7 @@
       <c r="C57" s="31"/>
       <c r="D57" s="11"/>
       <c r="E57" s="38" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5373,10 +5440,10 @@
         <v>81</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E59" s="80" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5403,7 +5470,7 @@
       <c r="C62" s="31"/>
       <c r="D62" s="11"/>
       <c r="E62" s="38" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5422,10 +5489,10 @@
         <v>82</v>
       </c>
       <c r="D64" s="21" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E64" s="80" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5435,7 +5502,7 @@
       </c>
       <c r="C65" s="24"/>
       <c r="D65" s="11" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E65" s="79"/>
     </row>
@@ -5445,7 +5512,7 @@
       <c r="C66" s="11"/>
       <c r="D66" s="11"/>
       <c r="E66" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5454,7 +5521,7 @@
       <c r="C67" s="24"/>
       <c r="D67" s="11"/>
       <c r="E67" s="11" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5470,7 +5537,7 @@
       <c r="C69" s="24"/>
       <c r="D69" s="11"/>
       <c r="E69" s="38" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5489,10 +5556,10 @@
         <v>83</v>
       </c>
       <c r="D71" s="23" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E71" s="80" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5502,7 +5569,7 @@
       </c>
       <c r="C72" s="31"/>
       <c r="D72" s="10" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E72" s="79"/>
     </row>
@@ -5514,7 +5581,7 @@
       <c r="C73" s="31"/>
       <c r="D73" s="10"/>
       <c r="E73" s="41" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5523,7 +5590,7 @@
       <c r="C74" s="31"/>
       <c r="D74" s="10"/>
       <c r="E74" s="41" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5532,7 +5599,7 @@
       <c r="C75" s="31"/>
       <c r="D75" s="10"/>
       <c r="E75" s="41" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5541,7 +5608,7 @@
       <c r="C76" s="31"/>
       <c r="D76" s="10"/>
       <c r="E76" s="41" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5560,10 +5627,10 @@
         <v>84</v>
       </c>
       <c r="D78" s="23" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E78" s="80" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5573,7 +5640,7 @@
       </c>
       <c r="C79" s="31"/>
       <c r="D79" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E79" s="79"/>
     </row>
@@ -5593,10 +5660,10 @@
         <v>85</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E81" s="79" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5623,7 +5690,7 @@
       <c r="C84" s="31"/>
       <c r="D84" s="10"/>
       <c r="E84" s="38" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5645,7 +5712,7 @@
         <v>49</v>
       </c>
       <c r="E86" s="80" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5655,7 +5722,7 @@
       </c>
       <c r="C87" s="31"/>
       <c r="D87" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E87" s="79"/>
     </row>
@@ -5674,7 +5741,7 @@
       <c r="C89" s="31"/>
       <c r="D89" s="10"/>
       <c r="E89" s="38" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5687,16 +5754,16 @@
     <row r="91" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="3"/>
       <c r="B91" s="32" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C91" s="43">
         <v>71</v>
       </c>
       <c r="D91" s="28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E91" s="21" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5704,7 +5771,7 @@
       <c r="B92" s="39"/>
       <c r="C92" s="44"/>
       <c r="D92" s="45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E92" s="14"/>
     </row>
@@ -5717,10 +5784,10 @@
         <v>86</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E93" s="46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5732,10 +5799,10 @@
         <v>87</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E94" s="11" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5747,10 +5814,10 @@
         <v>88</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E95" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5759,7 +5826,7 @@
       <c r="C96" s="24"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5775,7 +5842,7 @@
       <c r="C98" s="24"/>
       <c r="D98" s="6"/>
       <c r="E98" s="38" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5784,7 +5851,7 @@
       <c r="C99" s="24"/>
       <c r="D99" s="6"/>
       <c r="E99" s="38" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5793,7 +5860,7 @@
       <c r="C100" s="24"/>
       <c r="D100" s="6"/>
       <c r="E100" s="38" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5812,10 +5879,10 @@
         <v>90</v>
       </c>
       <c r="D102" s="48" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E102" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5831,7 +5898,7 @@
       <c r="C104" s="49"/>
       <c r="D104" s="50"/>
       <c r="E104" s="34" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5848,10 +5915,10 @@
         <v>100</v>
       </c>
       <c r="D106" s="28" t="s">
+        <v>446</v>
+      </c>
+      <c r="E106" s="77" t="s">
         <v>449</v>
-      </c>
-      <c r="E106" s="77" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5860,7 +5927,7 @@
       <c r="C107" s="74"/>
       <c r="D107" s="75"/>
       <c r="E107" s="78" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5876,7 +5943,7 @@
       <c r="C109" s="74"/>
       <c r="D109" s="75"/>
       <c r="E109" s="38" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5889,16 +5956,16 @@
     <row r="111" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111" s="3"/>
       <c r="B111" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C111" s="35">
         <v>3</v>
       </c>
       <c r="D111" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E111" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5908,7 +5975,7 @@
         <v>4</v>
       </c>
       <c r="D112" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E112" s="52"/>
     </row>
@@ -5919,7 +5986,7 @@
         <v>5</v>
       </c>
       <c r="D113" s="36" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E113" s="52"/>
     </row>
@@ -5930,7 +5997,7 @@
         <v>6</v>
       </c>
       <c r="D114" s="36" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E114" s="52"/>
     </row>
@@ -5941,7 +6008,7 @@
         <v>7</v>
       </c>
       <c r="D115" s="36" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E115" s="52"/>
     </row>
@@ -5952,7 +6019,7 @@
         <v>8</v>
       </c>
       <c r="D116" s="36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E116" s="52"/>
     </row>
@@ -5963,7 +6030,7 @@
         <v>9</v>
       </c>
       <c r="D117" s="36" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E117" s="52"/>
     </row>
@@ -5974,7 +6041,7 @@
         <v>10</v>
       </c>
       <c r="D118" s="36" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E118" s="52"/>
     </row>
@@ -5985,7 +6052,7 @@
         <v>16</v>
       </c>
       <c r="D119" s="36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E119" s="52"/>
     </row>
@@ -5996,7 +6063,7 @@
         <v>18</v>
       </c>
       <c r="D120" s="36" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E120" s="52"/>
     </row>
@@ -6007,7 +6074,7 @@
         <v>19</v>
       </c>
       <c r="D121" s="36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E121" s="52"/>
     </row>
@@ -6018,7 +6085,7 @@
         <v>20</v>
       </c>
       <c r="D122" s="36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E122" s="53"/>
     </row>
@@ -6035,7 +6102,7 @@
         <v>61</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D124" s="54"/>
       <c r="E124" s="3"/>
@@ -6050,16 +6117,16 @@
     <row r="126" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A126" s="3"/>
       <c r="B126" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C126" s="19" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D126" s="9" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E126" s="9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6068,13 +6135,13 @@
         <v>55</v>
       </c>
       <c r="C127" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="D127" s="55" t="s">
         <v>240</v>
       </c>
-      <c r="D127" s="55" t="s">
-        <v>241</v>
-      </c>
       <c r="E127" s="9" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6082,23 +6149,23 @@
       <c r="B128" s="56"/>
       <c r="C128" s="24"/>
       <c r="D128" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E128" s="58" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A129" s="3"/>
       <c r="B129" s="56"/>
       <c r="C129" s="59" t="s">
+        <v>242</v>
+      </c>
+      <c r="D129" s="55" t="s">
         <v>243</v>
       </c>
-      <c r="D129" s="55" t="s">
-        <v>244</v>
-      </c>
       <c r="E129" s="9" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6106,10 +6173,10 @@
       <c r="B130" s="31"/>
       <c r="C130" s="60"/>
       <c r="D130" s="57" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E130" s="9" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6117,10 +6184,10 @@
       <c r="B131" s="31"/>
       <c r="C131" s="60"/>
       <c r="D131" s="61" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E131" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6128,10 +6195,10 @@
       <c r="B132" s="31"/>
       <c r="C132" s="56"/>
       <c r="D132" s="21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E132" s="81" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6146,10 +6213,10 @@
       <c r="B134" s="31"/>
       <c r="C134" s="60"/>
       <c r="D134" s="62" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E134" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6159,10 +6226,10 @@
         <v>4</v>
       </c>
       <c r="D135" s="62" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E135" s="9" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6170,10 +6237,10 @@
       <c r="B136" s="31"/>
       <c r="C136" s="24"/>
       <c r="D136" s="57" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E136" s="9" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6181,10 +6248,10 @@
       <c r="B137" s="31"/>
       <c r="C137" s="24"/>
       <c r="D137" s="57" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E137" s="9" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6192,10 +6259,10 @@
       <c r="B138" s="31"/>
       <c r="C138" s="24"/>
       <c r="D138" s="57" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E138" s="9" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6203,10 +6270,10 @@
       <c r="B139" s="31"/>
       <c r="C139" s="24"/>
       <c r="D139" s="57" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E139" s="9" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6214,10 +6281,10 @@
       <c r="B140" s="31"/>
       <c r="C140" s="24"/>
       <c r="D140" s="57" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E140" s="9" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6225,10 +6292,10 @@
       <c r="B141" s="31"/>
       <c r="C141" s="24"/>
       <c r="D141" s="57" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E141" s="9" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6236,10 +6303,10 @@
       <c r="B142" s="31"/>
       <c r="C142" s="24"/>
       <c r="D142" s="57" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E142" s="9" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6247,10 +6314,10 @@
       <c r="B143" s="56"/>
       <c r="C143" s="24"/>
       <c r="D143" s="57" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E143" s="9" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6258,10 +6325,10 @@
       <c r="B144" s="56"/>
       <c r="C144" s="24"/>
       <c r="D144" s="57" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E144" s="9" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6269,10 +6336,10 @@
       <c r="B145" s="56"/>
       <c r="C145" s="24"/>
       <c r="D145" s="57" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E145" s="9" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6280,10 +6347,10 @@
       <c r="B146" s="56"/>
       <c r="C146" s="24"/>
       <c r="D146" s="57" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E146" s="9" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6291,10 +6358,10 @@
       <c r="B147" s="56"/>
       <c r="C147" s="24"/>
       <c r="D147" s="57" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E147" s="9" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6302,10 +6369,10 @@
       <c r="B148" s="56"/>
       <c r="C148" s="24"/>
       <c r="D148" s="57" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E148" s="9" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6313,10 +6380,10 @@
       <c r="B149" s="56"/>
       <c r="C149" s="24"/>
       <c r="D149" s="57" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E149" s="9" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6324,10 +6391,10 @@
       <c r="B150" s="56"/>
       <c r="C150" s="24"/>
       <c r="D150" s="57" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E150" s="9" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6335,10 +6402,10 @@
       <c r="B151" s="56"/>
       <c r="C151" s="24"/>
       <c r="D151" s="57" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E151" s="9" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6346,10 +6413,10 @@
       <c r="B152" s="56"/>
       <c r="C152" s="24"/>
       <c r="D152" s="57" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E152" s="9" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6357,23 +6424,23 @@
       <c r="B153" s="56"/>
       <c r="C153" s="24"/>
       <c r="D153" s="57" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E153" s="9" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A154" s="3"/>
       <c r="B154" s="56"/>
       <c r="C154" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="D154" s="57" t="s">
         <v>268</v>
       </c>
-      <c r="D154" s="57" t="s">
-        <v>269</v>
-      </c>
       <c r="E154" s="9" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6381,10 +6448,10 @@
       <c r="B155" s="56"/>
       <c r="C155" s="24"/>
       <c r="D155" s="57" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E155" s="9" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6392,10 +6459,10 @@
       <c r="B156" s="63"/>
       <c r="C156" s="30"/>
       <c r="D156" s="57" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E156" s="9" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -6411,7 +6478,7 @@
         <v>61</v>
       </c>
       <c r="C158" s="64" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D158" s="54"/>
       <c r="E158" s="3"/>
@@ -6426,16 +6493,16 @@
     <row r="160" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A160" s="3"/>
       <c r="B160" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C160" s="20" t="s">
         <v>5</v>
       </c>
       <c r="D160" s="9" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E160" s="9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6450,7 +6517,7 @@
         <v>6</v>
       </c>
       <c r="E161" s="65" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6463,7 +6530,7 @@
         <v>6</v>
       </c>
       <c r="E162" s="65" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6476,7 +6543,7 @@
         <v>6</v>
       </c>
       <c r="E163" s="65" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6489,7 +6556,7 @@
         <v>6</v>
       </c>
       <c r="E164" s="65" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6502,7 +6569,7 @@
         <v>6</v>
       </c>
       <c r="E165" s="65" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6528,7 +6595,7 @@
         <v>6</v>
       </c>
       <c r="E167" s="65" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6541,7 +6608,7 @@
         <v>6</v>
       </c>
       <c r="E168" s="9" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6593,7 +6660,7 @@
         <v>6</v>
       </c>
       <c r="E172" s="9" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6619,7 +6686,7 @@
         <v>6</v>
       </c>
       <c r="E174" s="9" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6632,7 +6699,7 @@
         <v>6</v>
       </c>
       <c r="E175" s="9" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6645,7 +6712,7 @@
         <v>6</v>
       </c>
       <c r="E176" s="9" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6658,7 +6725,7 @@
         <v>6</v>
       </c>
       <c r="E177" s="9" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6671,7 +6738,7 @@
         <v>179</v>
       </c>
       <c r="E178" s="67" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6684,7 +6751,7 @@
         <v>6</v>
       </c>
       <c r="E179" s="9" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6697,7 +6764,7 @@
         <v>6</v>
       </c>
       <c r="E180" s="9" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6710,7 +6777,7 @@
         <v>6</v>
       </c>
       <c r="E181" s="9" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6723,7 +6790,7 @@
         <v>6</v>
       </c>
       <c r="E182" s="9" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6736,7 +6803,7 @@
         <v>6</v>
       </c>
       <c r="E183" s="9" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6749,7 +6816,7 @@
         <v>6</v>
       </c>
       <c r="E184" s="9" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6762,7 +6829,7 @@
         <v>6</v>
       </c>
       <c r="E185" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6775,7 +6842,7 @@
         <v>6</v>
       </c>
       <c r="E186" s="9" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6788,7 +6855,7 @@
         <v>6</v>
       </c>
       <c r="E187" s="9" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6801,7 +6868,7 @@
         <v>6</v>
       </c>
       <c r="E188" s="9" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6814,7 +6881,7 @@
         <v>6</v>
       </c>
       <c r="E189" s="9" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6827,7 +6894,7 @@
         <v>6</v>
       </c>
       <c r="E190" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6840,7 +6907,7 @@
         <v>11</v>
       </c>
       <c r="E191" s="65" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6853,7 +6920,7 @@
         <v>11</v>
       </c>
       <c r="E192" s="65" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6866,7 +6933,7 @@
         <v>11</v>
       </c>
       <c r="E193" s="9" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6879,7 +6946,7 @@
         <v>11</v>
       </c>
       <c r="E194" s="67" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6892,7 +6959,7 @@
         <v>11</v>
       </c>
       <c r="E195" s="67" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6905,7 +6972,7 @@
         <v>11</v>
       </c>
       <c r="E196" s="67" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="197" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6918,7 +6985,7 @@
         <v>11</v>
       </c>
       <c r="E197" s="67" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="198" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6931,7 +6998,7 @@
         <v>11</v>
       </c>
       <c r="E198" s="67" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="199" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6944,7 +7011,7 @@
         <v>11</v>
       </c>
       <c r="E199" s="67" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="200" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6957,7 +7024,7 @@
         <v>11</v>
       </c>
       <c r="E200" s="67" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6970,7 +7037,7 @@
         <v>11</v>
       </c>
       <c r="E201" s="67" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6983,7 +7050,7 @@
         <v>11</v>
       </c>
       <c r="E202" s="67" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="203" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6996,7 +7063,7 @@
         <v>11</v>
       </c>
       <c r="E203" s="67" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -7009,7 +7076,7 @@
         <v>11</v>
       </c>
       <c r="E204" s="67" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="205" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -7022,7 +7089,7 @@
         <v>11</v>
       </c>
       <c r="E205" s="67" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="206" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -7035,7 +7102,7 @@
         <v>11</v>
       </c>
       <c r="E206" s="67" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="207" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -7048,7 +7115,7 @@
         <v>11</v>
       </c>
       <c r="E207" s="67" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="208" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -7061,7 +7128,7 @@
         <v>11</v>
       </c>
       <c r="E208" s="67" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="209" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -7074,7 +7141,7 @@
         <v>179</v>
       </c>
       <c r="E209" s="67" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="210" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -7087,25 +7154,25 @@
         <v>179</v>
       </c>
       <c r="E210" s="67" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="211" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A211" s="3"/>
       <c r="B211" s="24"/>
       <c r="C211" s="66" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D211" s="67" t="s">
         <v>179</v>
       </c>
       <c r="E211" s="67" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="212" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A212" s="3"/>
-      <c r="B212" s="30"/>
+      <c r="B212" s="24"/>
       <c r="C212" s="35" t="s">
         <v>66</v>
       </c>
@@ -7113,471 +7180,471 @@
         <v>6</v>
       </c>
       <c r="E212" s="65" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="213" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A213" s="3"/>
-      <c r="B213" s="19" t="s">
-        <v>274</v>
-      </c>
-      <c r="C213" s="66" t="s">
-        <v>10</v>
-      </c>
-      <c r="D213" s="67" t="s">
+      <c r="B213" s="30"/>
+      <c r="C213" s="35" t="s">
+        <v>477</v>
+      </c>
+      <c r="D213" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="E213" s="67" t="s">
-        <v>293</v>
+      <c r="E213" s="65" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="214" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A214" s="3"/>
-      <c r="B214" s="24"/>
+      <c r="B214" s="19" t="s">
+        <v>273</v>
+      </c>
       <c r="C214" s="66" t="s">
-        <v>108</v>
+        <v>10</v>
       </c>
       <c r="D214" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E214" s="67" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="215" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A215" s="3"/>
       <c r="B215" s="24"/>
       <c r="C215" s="66" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D215" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E215" s="67" t="s">
-        <v>411</v>
+        <v>293</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A216" s="3"/>
       <c r="B216" s="24"/>
       <c r="C216" s="66" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D216" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E216" s="67" t="s">
-        <v>295</v>
+        <v>409</v>
       </c>
     </row>
     <row r="217" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A217" s="3"/>
       <c r="B217" s="24"/>
       <c r="C217" s="66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D217" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E217" s="67" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="218" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A218" s="3"/>
       <c r="B218" s="24"/>
       <c r="C218" s="66" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D218" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E218" s="67" t="s">
-        <v>388</v>
+        <v>295</v>
       </c>
     </row>
     <row r="219" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A219" s="3"/>
       <c r="B219" s="24"/>
       <c r="C219" s="66" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D219" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E219" s="67" t="s">
-        <v>412</v>
+        <v>386</v>
       </c>
     </row>
     <row r="220" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A220" s="3"/>
       <c r="B220" s="24"/>
       <c r="C220" s="66" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D220" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E220" s="67" t="s">
-        <v>279</v>
+        <v>410</v>
       </c>
     </row>
     <row r="221" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A221" s="3"/>
       <c r="B221" s="24"/>
       <c r="C221" s="66" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D221" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E221" s="67" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
     </row>
     <row r="222" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A222" s="3"/>
       <c r="B222" s="24"/>
       <c r="C222" s="66" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D222" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E222" s="67" t="s">
-        <v>413</v>
+        <v>296</v>
       </c>
     </row>
     <row r="223" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A223" s="3"/>
       <c r="B223" s="24"/>
       <c r="C223" s="66" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D223" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E223" s="67" t="s">
-        <v>280</v>
+        <v>411</v>
       </c>
     </row>
     <row r="224" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A224" s="3"/>
       <c r="B224" s="24"/>
       <c r="C224" s="66" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D224" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E224" s="67" t="s">
-        <v>435</v>
+        <v>279</v>
       </c>
     </row>
     <row r="225" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A225" s="3"/>
       <c r="B225" s="24"/>
       <c r="C225" s="66" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D225" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E225" s="67" t="s">
-        <v>414</v>
+        <v>432</v>
       </c>
     </row>
     <row r="226" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A226" s="3"/>
       <c r="B226" s="24"/>
       <c r="C226" s="66" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D226" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E226" s="67" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="227" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A227" s="3"/>
       <c r="B227" s="24"/>
       <c r="C227" s="66" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D227" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E227" s="67" t="s">
-        <v>298</v>
+        <v>413</v>
       </c>
     </row>
     <row r="228" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A228" s="3"/>
       <c r="B228" s="24"/>
       <c r="C228" s="66" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D228" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E228" s="67" t="s">
-        <v>281</v>
+        <v>297</v>
       </c>
     </row>
     <row r="229" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A229" s="3"/>
       <c r="B229" s="24"/>
       <c r="C229" s="66" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D229" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E229" s="67" t="s">
-        <v>299</v>
+        <v>280</v>
       </c>
     </row>
     <row r="230" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A230" s="3"/>
       <c r="B230" s="24"/>
       <c r="C230" s="66" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D230" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E230" s="67" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="231" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A231" s="3"/>
       <c r="B231" s="24"/>
       <c r="C231" s="66" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D231" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E231" s="67" t="s">
-        <v>282</v>
+        <v>299</v>
       </c>
     </row>
     <row r="232" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A232" s="3"/>
       <c r="B232" s="24"/>
       <c r="C232" s="66" t="s">
-        <v>12</v>
+        <v>125</v>
       </c>
       <c r="D232" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E232" s="67" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="233" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A233" s="33"/>
-      <c r="B233" s="2"/>
-      <c r="C233" s="70" t="s">
+      <c r="A233" s="3"/>
+      <c r="B233" s="24"/>
+      <c r="C233" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="D233" s="67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E233" s="67" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A234" s="33"/>
+      <c r="B234" s="2"/>
+      <c r="C234" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="D233" s="65" t="s">
+      <c r="D234" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="E233" s="65" t="s">
+      <c r="E234" s="65" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="234" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A234" s="3"/>
-      <c r="B234" s="24"/>
-      <c r="C234" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D234" s="65" t="s">
-        <v>11</v>
-      </c>
-      <c r="E234" s="65" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="235" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A235" s="3"/>
       <c r="B235" s="24"/>
       <c r="C235" s="35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D235" s="65" t="s">
         <v>11</v>
       </c>
       <c r="E235" s="65" t="s">
-        <v>416</v>
+        <v>300</v>
       </c>
     </row>
     <row r="236" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A236" s="3"/>
       <c r="B236" s="24"/>
       <c r="C236" s="35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D236" s="65" t="s">
         <v>11</v>
       </c>
       <c r="E236" s="65" t="s">
-        <v>302</v>
+        <v>414</v>
       </c>
     </row>
     <row r="237" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A237" s="3"/>
       <c r="B237" s="24"/>
       <c r="C237" s="35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D237" s="65" t="s">
         <v>11</v>
       </c>
       <c r="E237" s="65" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="238" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A238" s="3"/>
       <c r="B238" s="24"/>
       <c r="C238" s="35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D238" s="65" t="s">
         <v>11</v>
       </c>
       <c r="E238" s="65" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="239" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A239" s="3"/>
       <c r="B239" s="24"/>
       <c r="C239" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D239" s="65" t="s">
         <v>11</v>
       </c>
       <c r="E239" s="65" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="240" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A240" s="3"/>
       <c r="B240" s="24"/>
-      <c r="C240" s="66" t="s">
-        <v>20</v>
-      </c>
-      <c r="D240" s="67" t="s">
-        <v>25</v>
-      </c>
-      <c r="E240" s="67" t="s">
-        <v>460</v>
+      <c r="C240" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D240" s="65" t="s">
+        <v>11</v>
+      </c>
+      <c r="E240" s="65" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="241" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A241" s="3"/>
       <c r="B241" s="24"/>
       <c r="C241" s="66" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D241" s="67" t="s">
         <v>25</v>
       </c>
       <c r="E241" s="67" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="242" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A242" s="3"/>
       <c r="B242" s="24"/>
       <c r="C242" s="66" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D242" s="67" t="s">
         <v>25</v>
       </c>
       <c r="E242" s="67" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="243" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A243" s="3"/>
       <c r="B243" s="24"/>
       <c r="C243" s="66" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D243" s="67" t="s">
         <v>25</v>
       </c>
       <c r="E243" s="67" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="244" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A244" s="3"/>
       <c r="B244" s="24"/>
       <c r="C244" s="66" t="s">
-        <v>147</v>
+        <v>24</v>
       </c>
       <c r="D244" s="67" t="s">
         <v>25</v>
       </c>
       <c r="E244" s="67" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="245" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A245" s="3"/>
       <c r="B245" s="24"/>
       <c r="C245" s="66" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D245" s="67" t="s">
         <v>25</v>
       </c>
       <c r="E245" s="67" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="246" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A246" s="3"/>
       <c r="B246" s="24"/>
-      <c r="C246" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D246" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E246" s="9" t="s">
-        <v>199</v>
+      <c r="C246" s="66" t="s">
+        <v>148</v>
+      </c>
+      <c r="D246" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="E246" s="67" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="247" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A247" s="3"/>
       <c r="B247" s="24"/>
-      <c r="C247" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D247" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E247" s="9" t="s">
-        <v>200</v>
+      <c r="C247" s="66" t="s">
+        <v>472</v>
+      </c>
+      <c r="D247" s="67" t="s">
+        <v>473</v>
+      </c>
+      <c r="E247" s="67" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="248" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A248" s="3"/>
       <c r="B248" s="24"/>
       <c r="C248" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D248" s="9" t="s">
         <v>21</v>
@@ -7590,697 +7657,775 @@
       <c r="A249" s="3"/>
       <c r="B249" s="24"/>
       <c r="C249" s="20" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="D249" s="9" t="s">
         <v>21</v>
       </c>
       <c r="E249" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="250" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A250" s="3"/>
       <c r="B250" s="24"/>
       <c r="C250" s="20" t="s">
-        <v>127</v>
+        <v>28</v>
       </c>
       <c r="D250" s="9" t="s">
         <v>21</v>
       </c>
       <c r="E250" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="251" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A251" s="3"/>
-      <c r="B251" s="30"/>
+      <c r="B251" s="24"/>
       <c r="C251" s="20" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
       <c r="D251" s="9" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E251" s="9" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
     </row>
     <row r="252" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A252" s="3"/>
-      <c r="B252" s="19" t="s">
-        <v>55</v>
-      </c>
+      <c r="B252" s="24"/>
       <c r="C252" s="20" t="s">
-        <v>30</v>
+        <v>127</v>
       </c>
       <c r="D252" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E252" s="9" t="s">
-        <v>150</v>
+        <v>197</v>
       </c>
     </row>
     <row r="253" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A253" s="3"/>
-      <c r="B253" s="24"/>
+      <c r="B253" s="30"/>
       <c r="C253" s="20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D253" s="9" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E253" s="9" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
     </row>
     <row r="254" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A254" s="3"/>
-      <c r="B254" s="24"/>
+      <c r="B254" s="19" t="s">
+        <v>55</v>
+      </c>
       <c r="C254" s="20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D254" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E254" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="255" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A255" s="3"/>
       <c r="B255" s="24"/>
       <c r="C255" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D255" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E255" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="256" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A256" s="3"/>
       <c r="B256" s="24"/>
       <c r="C256" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D256" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E256" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="257" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A257" s="3"/>
       <c r="B257" s="24"/>
       <c r="C257" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D257" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E257" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="258" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A258" s="3"/>
       <c r="B258" s="24"/>
       <c r="C258" s="20" t="s">
-        <v>128</v>
+        <v>34</v>
       </c>
       <c r="D258" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E258" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="259" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A259" s="3"/>
       <c r="B259" s="24"/>
       <c r="C259" s="20" t="s">
-        <v>129</v>
+        <v>35</v>
       </c>
       <c r="D259" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E259" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="260" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A260" s="3"/>
       <c r="B260" s="24"/>
       <c r="C260" s="20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D260" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E260" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="261" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A261" s="3"/>
       <c r="B261" s="24"/>
       <c r="C261" s="20" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D261" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E261" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="262" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A262" s="3"/>
       <c r="B262" s="24"/>
       <c r="C262" s="20" t="s">
-        <v>36</v>
+        <v>130</v>
       </c>
       <c r="D262" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E262" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="263" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A263" s="3"/>
       <c r="B263" s="24"/>
       <c r="C263" s="20" t="s">
-        <v>37</v>
+        <v>131</v>
       </c>
       <c r="D263" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E263" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="264" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A264" s="3"/>
       <c r="B264" s="24"/>
       <c r="C264" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D264" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E264" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="265" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A265" s="3"/>
       <c r="B265" s="24"/>
       <c r="C265" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D265" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E265" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="266" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A266" s="3"/>
       <c r="B266" s="24"/>
       <c r="C266" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D266" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E266" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="267" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A267" s="3"/>
       <c r="B267" s="24"/>
       <c r="C267" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D267" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E267" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="268" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A268" s="3"/>
       <c r="B268" s="24"/>
       <c r="C268" s="20" t="s">
-        <v>149</v>
+        <v>40</v>
       </c>
       <c r="D268" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E268" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="269" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A269" s="3"/>
       <c r="B269" s="24"/>
       <c r="C269" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D269" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E269" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="270" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A270" s="3"/>
       <c r="B270" s="24"/>
       <c r="C270" s="20" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
       <c r="D270" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E270" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="271" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A271" s="3"/>
       <c r="B271" s="24"/>
       <c r="C271" s="20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D271" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E271" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="272" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A272" s="3"/>
       <c r="B272" s="24"/>
       <c r="C272" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D272" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E272" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="273" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A273" s="3"/>
       <c r="B273" s="24"/>
       <c r="C273" s="20" t="s">
-        <v>132</v>
+        <v>44</v>
       </c>
       <c r="D273" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E273" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="274" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A274" s="3"/>
       <c r="B274" s="24"/>
       <c r="C274" s="20" t="s">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="D274" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E274" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="275" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A275" s="3"/>
       <c r="B275" s="24"/>
       <c r="C275" s="20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D275" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E275" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="276" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A276" s="3"/>
       <c r="B276" s="24"/>
       <c r="C276" s="20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D276" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E276" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="277" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A277" s="3"/>
       <c r="B277" s="24"/>
       <c r="C277" s="20" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D277" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E277" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="278" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A278" s="3"/>
       <c r="B278" s="24"/>
-      <c r="C278" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="D278" s="65" t="s">
+      <c r="C278" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="D278" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E278" s="65" t="s">
-        <v>176</v>
+      <c r="E278" s="9" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="279" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A279" s="3"/>
-      <c r="B279" s="30"/>
-      <c r="C279" s="35" t="s">
+      <c r="B279" s="24"/>
+      <c r="C279" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D279" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E279" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A280" s="3"/>
+      <c r="B280" s="24"/>
+      <c r="C280" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="D280" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="E280" s="65" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A281" s="3"/>
+      <c r="B281" s="30"/>
+      <c r="C281" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="D279" s="65" t="s">
+      <c r="D281" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="E279" s="65" t="s">
+      <c r="E281" s="65" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="280" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A280" s="3"/>
-      <c r="B280" s="6"/>
-      <c r="C280" s="6"/>
-      <c r="D280" s="6"/>
-      <c r="E280" s="6"/>
-    </row>
-    <row r="281" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A281" s="3"/>
-      <c r="B281" s="68" t="s">
+    <row r="282" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A282" s="3"/>
+      <c r="B282" s="6"/>
+      <c r="C282" s="6"/>
+      <c r="D282" s="6"/>
+      <c r="E282" s="6"/>
+    </row>
+    <row r="283" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A283" s="3"/>
+      <c r="B283" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="C281" s="64" t="s">
-        <v>417</v>
-      </c>
-      <c r="D281" s="54"/>
-      <c r="E281" s="3"/>
-    </row>
-    <row r="282" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A282" s="3"/>
-      <c r="B282" s="3"/>
-      <c r="C282" s="3"/>
-      <c r="D282" s="3"/>
-      <c r="E282" s="3"/>
-    </row>
-    <row r="283" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A283" s="3"/>
-      <c r="B283" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="C283" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D283" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="E283" s="9" t="s">
-        <v>356</v>
-      </c>
+      <c r="C283" s="64" t="s">
+        <v>415</v>
+      </c>
+      <c r="D283" s="54"/>
+      <c r="E283" s="3"/>
     </row>
     <row r="284" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A284" s="3"/>
-      <c r="B284" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C284" s="35" t="s">
-        <v>212</v>
-      </c>
-      <c r="D284" s="67" t="s">
-        <v>180</v>
-      </c>
-      <c r="E284" s="65" t="s">
-        <v>306</v>
-      </c>
+      <c r="B284" s="3"/>
+      <c r="C284" s="3"/>
+      <c r="D284" s="3"/>
+      <c r="E284" s="3"/>
     </row>
     <row r="285" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A285" s="3"/>
-      <c r="B285" s="24"/>
-      <c r="C285" s="69" t="s">
-        <v>182</v>
-      </c>
-      <c r="D285" s="58" t="s">
-        <v>180</v>
-      </c>
-      <c r="E285" s="67" t="s">
-        <v>307</v>
+      <c r="B285" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="C285" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D285" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E285" s="9" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="286" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A286" s="3"/>
-      <c r="B286" s="11"/>
-      <c r="C286" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D286" s="58" t="s">
+      <c r="B286" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C286" s="35" t="s">
+        <v>211</v>
+      </c>
+      <c r="D286" s="67" t="s">
         <v>180</v>
       </c>
-      <c r="E286" s="9" t="s">
-        <v>389</v>
+      <c r="E286" s="65" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="287" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A287" s="3"/>
-      <c r="B287" s="11"/>
-      <c r="C287" s="25" t="s">
-        <v>184</v>
+      <c r="B287" s="24"/>
+      <c r="C287" s="69" t="s">
+        <v>182</v>
       </c>
       <c r="D287" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="E287" s="9" t="s">
-        <v>418</v>
+      <c r="E287" s="67" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="288" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A288" s="3"/>
       <c r="B288" s="11"/>
       <c r="C288" s="25" t="s">
-        <v>185</v>
+        <v>68</v>
       </c>
       <c r="D288" s="58" t="s">
         <v>180</v>
       </c>
       <c r="E288" s="9" t="s">
-        <v>419</v>
+        <v>387</v>
       </c>
     </row>
     <row r="289" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A289" s="3"/>
       <c r="B289" s="11"/>
       <c r="C289" s="25" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D289" s="58" t="s">
         <v>180</v>
       </c>
       <c r="E289" s="9" t="s">
-        <v>420</v>
+        <v>474</v>
       </c>
     </row>
     <row r="290" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A290" s="3"/>
       <c r="B290" s="11"/>
-      <c r="C290" s="70" t="s">
-        <v>213</v>
-      </c>
-      <c r="D290" s="67" t="s">
-        <v>214</v>
-      </c>
-      <c r="E290" s="65" t="s">
-        <v>308</v>
+      <c r="C290" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="D290" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="E290" s="9" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="291" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A291" s="3"/>
-      <c r="B291" s="24"/>
-      <c r="C291" s="70" t="s">
-        <v>196</v>
+      <c r="B291" s="11"/>
+      <c r="C291" s="25" t="s">
+        <v>193</v>
       </c>
       <c r="D291" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="E291" s="65" t="s">
-        <v>309</v>
+      <c r="E291" s="9" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="292" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A292" s="3"/>
-      <c r="B292" s="24"/>
-      <c r="C292" s="69" t="s">
-        <v>197</v>
-      </c>
-      <c r="D292" s="58" t="s">
-        <v>180</v>
-      </c>
-      <c r="E292" s="67" t="s">
-        <v>310</v>
+      <c r="B292" s="11"/>
+      <c r="C292" s="70" t="s">
+        <v>212</v>
+      </c>
+      <c r="D292" s="67" t="s">
+        <v>213</v>
+      </c>
+      <c r="E292" s="65" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="293" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A293" s="3"/>
-      <c r="B293" s="30"/>
+      <c r="B293" s="24"/>
       <c r="C293" s="70" t="s">
-        <v>183</v>
-      </c>
-      <c r="D293" s="67" t="s">
+        <v>195</v>
+      </c>
+      <c r="D293" s="58" t="s">
         <v>180</v>
       </c>
       <c r="E293" s="65" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A294" s="3"/>
+      <c r="B294" s="24"/>
+      <c r="C294" s="69" t="s">
+        <v>196</v>
+      </c>
+      <c r="D294" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="E294" s="67" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A295" s="3"/>
+      <c r="B295" s="24"/>
+      <c r="C295" s="70" t="s">
+        <v>476</v>
+      </c>
+      <c r="D295" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="E295" s="65" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="294" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A294" s="3"/>
-      <c r="B294" s="3"/>
-      <c r="C294" s="3"/>
-      <c r="D294" s="3"/>
-      <c r="E294" s="3"/>
-    </row>
-    <row r="295" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A295" s="3"/>
-      <c r="B295" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C295" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D295" s="3"/>
-      <c r="E295" s="3"/>
     </row>
     <row r="296" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A296" s="3"/>
-      <c r="B296" s="3"/>
-      <c r="C296" s="3"/>
-      <c r="D296" s="3"/>
-      <c r="E296" s="3"/>
+      <c r="B296" s="24"/>
+      <c r="C296" s="70" t="s">
+        <v>477</v>
+      </c>
+      <c r="D296" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="E296" s="65" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="297" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A297" s="3"/>
-      <c r="B297" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="C297" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D297" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="E297" s="9" t="s">
-        <v>48</v>
+      <c r="B297" s="24"/>
+      <c r="C297" s="70" t="s">
+        <v>484</v>
+      </c>
+      <c r="D297" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="E297" s="65" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="298" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A298" s="3"/>
-      <c r="B298" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C298" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="D298" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="E298" s="9" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="299" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B298" s="30"/>
+      <c r="C298" s="70" t="s">
+        <v>485</v>
+      </c>
+      <c r="D298" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="E298" s="65" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A299" s="3"/>
-      <c r="B299" s="24"/>
-      <c r="C299" s="35" t="s">
-        <v>215</v>
-      </c>
-      <c r="D299" s="35" t="s">
-        <v>216</v>
-      </c>
-      <c r="E299" s="65" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="300" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B299" s="3"/>
+      <c r="C299" s="3"/>
+      <c r="D299" s="3"/>
+      <c r="E299" s="3"/>
+    </row>
+    <row r="300" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A300" s="3"/>
-      <c r="B300" s="24"/>
-      <c r="C300" s="35" t="s">
-        <v>470</v>
-      </c>
-      <c r="D300" s="35" t="s">
-        <v>471</v>
-      </c>
-      <c r="E300" s="65" t="s">
-        <v>472</v>
-      </c>
+      <c r="B300" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C300" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D300" s="3"/>
+      <c r="E300" s="3"/>
     </row>
     <row r="301" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A301" s="3"/>
-      <c r="B301" s="11"/>
-      <c r="C301" s="35" t="s">
-        <v>189</v>
-      </c>
-      <c r="D301" s="65" t="s">
-        <v>312</v>
-      </c>
-      <c r="E301" s="65" t="s">
-        <v>190</v>
-      </c>
+      <c r="B301" s="3"/>
+      <c r="C301" s="3"/>
+      <c r="D301" s="3"/>
+      <c r="E301" s="3"/>
     </row>
     <row r="302" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A302" s="3"/>
-      <c r="B302" s="11"/>
-      <c r="C302" s="35" t="s">
-        <v>191</v>
-      </c>
-      <c r="D302" s="65" t="s">
-        <v>313</v>
-      </c>
-      <c r="E302" s="65" t="s">
-        <v>192</v>
+      <c r="B302" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="C302" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D302" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="E302" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="303" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A303" s="3"/>
-      <c r="B303" s="14"/>
-      <c r="C303" s="35" t="s">
-        <v>193</v>
-      </c>
-      <c r="D303" s="65" t="s">
-        <v>314</v>
-      </c>
-      <c r="E303" s="65" t="s">
-        <v>292</v>
+      <c r="B303" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C303" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D303" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="E303" s="9" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A304" s="3"/>
+      <c r="B304" s="24"/>
+      <c r="C304" s="35" t="s">
+        <v>214</v>
+      </c>
+      <c r="D304" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="E304" s="65" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A305" s="3"/>
+      <c r="B305" s="24"/>
+      <c r="C305" s="35" t="s">
+        <v>467</v>
+      </c>
+      <c r="D305" s="35" t="s">
+        <v>468</v>
+      </c>
+      <c r="E305" s="65" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A306" s="3"/>
+      <c r="B306" s="24"/>
+      <c r="C306" s="35" t="s">
+        <v>482</v>
+      </c>
+      <c r="D306" s="65" t="s">
+        <v>481</v>
+      </c>
+      <c r="E306" s="65" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A307" s="3"/>
+      <c r="B307" s="11"/>
+      <c r="C307" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="D307" s="65" t="s">
+        <v>310</v>
+      </c>
+      <c r="E307" s="65" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A308" s="3"/>
+      <c r="B308" s="11"/>
+      <c r="C308" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="D308" s="65" t="s">
+        <v>311</v>
+      </c>
+      <c r="E308" s="65" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A309" s="3"/>
+      <c r="B309" s="14"/>
+      <c r="C309" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="D309" s="65" t="s">
+        <v>312</v>
+      </c>
+      <c r="E309" s="65" t="s">
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -8305,9 +8450,9 @@
     <brk id="47" max="16383" man="1"/>
     <brk id="110" max="16383" man="1"/>
     <brk id="157" max="16383" man="1"/>
-    <brk id="212" max="4" man="1"/>
-    <brk id="251" max="4" man="1"/>
-    <brk id="280" max="16383" man="1"/>
+    <brk id="213" max="4" man="1"/>
+    <brk id="253" max="4" man="1"/>
+    <brk id="282" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add: Add ammeter function
</commit_message>
<xml_diff>
--- a/doc/ATCFS Specifications.xlsx
+++ b/doc/ATCFS Specifications.xlsx
@@ -10,15 +10,15 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$310</definedName>
-    <definedName name="subject" localSheetId="0">Sheet1!$C$285</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$330</definedName>
+    <definedName name="subject" localSheetId="0">Sheet1!$C$291</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="514">
   <si>
     <t>Map</t>
     <phoneticPr fontId="2"/>
@@ -3807,7 +3807,38 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>電流値[A * 1000] (experimental)</t>
+    <t>7 (テンキーではない)</t>
+  </si>
+  <si>
+    <t>ATS I</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>手元灯</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ats63</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ats64</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>手元灯スイッチの押下音</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>手元灯スイッチの開放音</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ワイパーの速度調節スイッチ</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>電流値[A * 1000] (力行: +, ブレーキ: -)</t>
     <rPh sb="0" eb="2">
       <t>デンリュウ</t>
     </rPh>
@@ -3817,34 +3848,225 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>7 (テンキーではない)</t>
-  </si>
-  <si>
-    <t>ATS I</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>手元灯</t>
+    <t>ats207</t>
+  </si>
+  <si>
+    <t>電流値[A * 1000] (力行およびブレーキ: +)</t>
+    <rPh sb="0" eb="2">
+      <t>デンリュウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>アタイ</t>
+    </rPh>
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>ats63</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>ats64</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>手元灯スイッチの押下音</t>
+    <t>ats208</t>
+  </si>
+  <si>
+    <t>電流値[A]の負号</t>
+    <rPh sb="0" eb="2">
+      <t>デンリュウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>フゴウ</t>
+    </rPh>
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>手元灯スイッチの開放音</t>
+    <t>ats209</t>
+  </si>
+  <si>
+    <t>ats210</t>
+  </si>
+  <si>
+    <t>ats211</t>
+  </si>
+  <si>
+    <t>ats212</t>
+  </si>
+  <si>
+    <t>電流値[A]の百の位</t>
+    <rPh sb="0" eb="2">
+      <t>デンリュウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ヒャク</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>クライ</t>
+    </rPh>
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>ワイパーの速度調節スイッチ</t>
+    <t>電流値[A]の十の位</t>
+    <rPh sb="0" eb="2">
+      <t>デンリュウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ジュウ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>クライ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>電流値[A]の一の位</t>
+    <rPh sb="0" eb="2">
+      <t>デンリュウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>イチ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>クライ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>電流値[A]の小数第一位</t>
+    <rPh sb="0" eb="2">
+      <t>デンリュウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ショウスウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ダイイチ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>イ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Notch\Notch.txt (For OpenBVE)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Current</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>力行の電流テーブル(空車)ファイルへの相対パス</t>
+    <rPh sb="0" eb="1">
+      <t>リキ</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>ギョウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Brake</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ブレーキの電流テーブル(空車)ファイルへの相対パス</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>電流テーブル(空車) (For OpenBVE)</t>
+    <rPh sb="0" eb="2">
+      <t>デンリュウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>クウシャ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>記述方法</t>
+    <rPh sb="0" eb="2">
+      <t>キジュツ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ホウホウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>2行目以降は、1列目に列車速度[km/h]を昇順で記述してください。値の間隔は一定である必要はありません。</t>
+    <rPh sb="1" eb="3">
+      <t>ギョウメ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>イコウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ただし、定義できる特性曲線の本数はノッチ1段あたり1本です。</t>
+    <rPh sb="4" eb="6">
+      <t>テイギ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>トクセイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>キョクセン</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ホンスウ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ダン</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>ホン</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Current</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>2列目以降に主電動機電流[A]を記述してください。1つの列が1本の特性曲線を表し、2つの値の間は線形補間されます。</t>
+    <rPh sb="28" eb="29">
+      <t>レツ</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>ホン</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>トクセイ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>キョクセン</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>アラワ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>1行目にヘッダーとしてTrainSpeed,Stage1,Stage2,…,StageNのようにを記述してください。(N = ノッチ段数)</t>
+    <rPh sb="1" eb="3">
+      <t>ギョウメ</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>ダンスウ</t>
+    </rPh>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -3852,7 +4074,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1"/>
@@ -3924,6 +4146,13 @@
       <family val="3"/>
       <charset val="128"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4246,7 +4475,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4484,6 +4713,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -4495,6 +4730,33 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4800,10 +5062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E309"/>
+  <dimension ref="A1:E329"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A277" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A291" sqref="A291"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A311" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B327" sqref="B327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -5379,7 +5641,7 @@
       <c r="D52" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="E52" s="80" t="s">
+      <c r="E52" s="82" t="s">
         <v>272</v>
       </c>
     </row>
@@ -5390,14 +5652,14 @@
       </c>
       <c r="C53" s="31"/>
       <c r="D53" s="11"/>
-      <c r="E53" s="79"/>
+      <c r="E53" s="81"/>
     </row>
     <row r="54" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="3"/>
       <c r="B54" s="31"/>
       <c r="C54" s="31"/>
       <c r="D54" s="11"/>
-      <c r="E54" s="79" t="s">
+      <c r="E54" s="81" t="s">
         <v>326</v>
       </c>
     </row>
@@ -5406,7 +5668,7 @@
       <c r="B55" s="31"/>
       <c r="C55" s="31"/>
       <c r="D55" s="11"/>
-      <c r="E55" s="79"/>
+      <c r="E55" s="81"/>
     </row>
     <row r="56" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="3"/>
@@ -5442,7 +5704,7 @@
       <c r="D59" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="E59" s="80" t="s">
+      <c r="E59" s="82" t="s">
         <v>328</v>
       </c>
     </row>
@@ -5453,7 +5715,7 @@
       </c>
       <c r="C60" s="31"/>
       <c r="D60" s="11"/>
-      <c r="E60" s="79"/>
+      <c r="E60" s="81"/>
     </row>
     <row r="61" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="3"/>
@@ -5491,7 +5753,7 @@
       <c r="D64" s="21" t="s">
         <v>330</v>
       </c>
-      <c r="E64" s="80" t="s">
+      <c r="E64" s="82" t="s">
         <v>331</v>
       </c>
     </row>
@@ -5504,7 +5766,7 @@
       <c r="D65" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="E65" s="79"/>
+      <c r="E65" s="81"/>
     </row>
     <row r="66" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="3"/>
@@ -5558,7 +5820,7 @@
       <c r="D71" s="23" t="s">
         <v>335</v>
       </c>
-      <c r="E71" s="80" t="s">
+      <c r="E71" s="82" t="s">
         <v>336</v>
       </c>
     </row>
@@ -5571,7 +5833,7 @@
       <c r="D72" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="E72" s="79"/>
+      <c r="E72" s="81"/>
     </row>
     <row r="73" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="3"/>
@@ -5629,7 +5891,7 @@
       <c r="D78" s="23" t="s">
         <v>335</v>
       </c>
-      <c r="E78" s="80" t="s">
+      <c r="E78" s="82" t="s">
         <v>338</v>
       </c>
     </row>
@@ -5642,7 +5904,7 @@
       <c r="D79" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="E79" s="79"/>
+      <c r="E79" s="81"/>
     </row>
     <row r="80" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="3"/>
@@ -5662,7 +5924,7 @@
       <c r="D81" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="E81" s="79" t="s">
+      <c r="E81" s="81" t="s">
         <v>340</v>
       </c>
     </row>
@@ -5673,7 +5935,7 @@
       </c>
       <c r="C82" s="31"/>
       <c r="D82" s="11"/>
-      <c r="E82" s="79"/>
+      <c r="E82" s="81"/>
     </row>
     <row r="83" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="3"/>
@@ -5711,7 +5973,7 @@
       <c r="D86" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="E86" s="80" t="s">
+      <c r="E86" s="82" t="s">
         <v>229</v>
       </c>
     </row>
@@ -5724,7 +5986,7 @@
       <c r="D87" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="E87" s="79"/>
+      <c r="E87" s="81"/>
     </row>
     <row r="88" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="3"/>
@@ -6197,7 +6459,7 @@
       <c r="D132" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="E132" s="81" t="s">
+      <c r="E132" s="83" t="s">
         <v>404</v>
       </c>
     </row>
@@ -6206,7 +6468,7 @@
       <c r="B133" s="31"/>
       <c r="C133" s="56"/>
       <c r="D133" s="14"/>
-      <c r="E133" s="82"/>
+      <c r="E133" s="84"/>
     </row>
     <row r="134" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A134" s="3"/>
@@ -7637,796 +7899,981 @@
         <v>473</v>
       </c>
       <c r="E247" s="67" t="s">
-        <v>480</v>
+        <v>488</v>
       </c>
     </row>
     <row r="248" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A248" s="3"/>
       <c r="B248" s="24"/>
-      <c r="C248" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D248" s="9" t="s">
+      <c r="C248" s="66" t="s">
+        <v>489</v>
+      </c>
+      <c r="D248" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="E248" s="9" t="s">
-        <v>198</v>
+      <c r="E248" s="67" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="249" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A249" s="3"/>
       <c r="B249" s="24"/>
-      <c r="C249" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D249" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E249" s="9" t="s">
-        <v>199</v>
+      <c r="C249" s="66" t="s">
+        <v>491</v>
+      </c>
+      <c r="D249" s="67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E249" s="67" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="250" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A250" s="3"/>
       <c r="B250" s="24"/>
-      <c r="C250" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D250" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E250" s="9" t="s">
-        <v>197</v>
+      <c r="C250" s="66" t="s">
+        <v>493</v>
+      </c>
+      <c r="D250" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="E250" s="67" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="251" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A251" s="3"/>
       <c r="B251" s="24"/>
-      <c r="C251" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="D251" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E251" s="9" t="s">
-        <v>197</v>
+      <c r="C251" s="66" t="s">
+        <v>494</v>
+      </c>
+      <c r="D251" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="E251" s="67" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="252" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A252" s="3"/>
       <c r="B252" s="24"/>
-      <c r="C252" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="D252" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E252" s="9" t="s">
-        <v>197</v>
+      <c r="C252" s="66" t="s">
+        <v>495</v>
+      </c>
+      <c r="D252" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="E252" s="67" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="253" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A253" s="3"/>
-      <c r="B253" s="30"/>
-      <c r="C253" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D253" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E253" s="9" t="s">
-        <v>178</v>
+      <c r="B253" s="24"/>
+      <c r="C253" s="66" t="s">
+        <v>496</v>
+      </c>
+      <c r="D253" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="E253" s="67" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="254" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A254" s="3"/>
-      <c r="B254" s="19" t="s">
-        <v>55</v>
-      </c>
+      <c r="B254" s="24"/>
       <c r="C254" s="20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D254" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E254" s="9" t="s">
-        <v>150</v>
+        <v>198</v>
       </c>
     </row>
     <row r="255" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A255" s="3"/>
       <c r="B255" s="24"/>
       <c r="C255" s="20" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D255" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E255" s="9" t="s">
-        <v>151</v>
+        <v>199</v>
       </c>
     </row>
     <row r="256" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A256" s="3"/>
       <c r="B256" s="24"/>
       <c r="C256" s="20" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D256" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E256" s="9" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="257" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A257" s="3"/>
       <c r="B257" s="24"/>
       <c r="C257" s="20" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="D257" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E257" s="9" t="s">
-        <v>153</v>
+        <v>197</v>
       </c>
     </row>
     <row r="258" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A258" s="3"/>
       <c r="B258" s="24"/>
       <c r="C258" s="20" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="D258" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E258" s="9" t="s">
-        <v>154</v>
+        <v>197</v>
       </c>
     </row>
     <row r="259" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A259" s="3"/>
-      <c r="B259" s="24"/>
+      <c r="B259" s="30"/>
       <c r="C259" s="20" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D259" s="9" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E259" s="9" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
     </row>
     <row r="260" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A260" s="3"/>
-      <c r="B260" s="24"/>
+      <c r="B260" s="19" t="s">
+        <v>55</v>
+      </c>
       <c r="C260" s="20" t="s">
-        <v>128</v>
+        <v>30</v>
       </c>
       <c r="D260" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E260" s="9" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="261" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A261" s="3"/>
       <c r="B261" s="24"/>
       <c r="C261" s="20" t="s">
-        <v>129</v>
+        <v>31</v>
       </c>
       <c r="D261" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E261" s="9" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="262" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A262" s="3"/>
       <c r="B262" s="24"/>
       <c r="C262" s="20" t="s">
-        <v>130</v>
+        <v>32</v>
       </c>
       <c r="D262" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E262" s="9" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="263" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A263" s="3"/>
       <c r="B263" s="24"/>
       <c r="C263" s="20" t="s">
-        <v>131</v>
+        <v>33</v>
       </c>
       <c r="D263" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E263" s="9" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="264" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A264" s="3"/>
       <c r="B264" s="24"/>
       <c r="C264" s="20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D264" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E264" s="9" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="265" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A265" s="3"/>
       <c r="B265" s="24"/>
       <c r="C265" s="20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D265" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E265" s="9" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="266" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A266" s="3"/>
       <c r="B266" s="24"/>
       <c r="C266" s="20" t="s">
-        <v>38</v>
+        <v>128</v>
       </c>
       <c r="D266" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E266" s="9" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="267" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A267" s="3"/>
       <c r="B267" s="24"/>
       <c r="C267" s="20" t="s">
-        <v>39</v>
+        <v>129</v>
       </c>
       <c r="D267" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E267" s="9" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="268" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A268" s="3"/>
       <c r="B268" s="24"/>
       <c r="C268" s="20" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D268" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E268" s="9" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="269" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A269" s="3"/>
       <c r="B269" s="24"/>
       <c r="C269" s="20" t="s">
-        <v>41</v>
+        <v>131</v>
       </c>
       <c r="D269" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E269" s="9" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="270" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A270" s="3"/>
       <c r="B270" s="24"/>
       <c r="C270" s="20" t="s">
-        <v>149</v>
+        <v>36</v>
       </c>
       <c r="D270" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E270" s="9" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="271" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A271" s="3"/>
       <c r="B271" s="24"/>
       <c r="C271" s="20" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D271" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E271" s="9" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="272" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A272" s="3"/>
       <c r="B272" s="24"/>
       <c r="C272" s="20" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D272" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E272" s="9" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="273" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A273" s="3"/>
       <c r="B273" s="24"/>
       <c r="C273" s="20" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D273" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E273" s="9" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="274" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A274" s="3"/>
       <c r="B274" s="24"/>
       <c r="C274" s="20" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D274" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E274" s="9" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="275" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A275" s="3"/>
       <c r="B275" s="24"/>
       <c r="C275" s="20" t="s">
-        <v>132</v>
+        <v>41</v>
       </c>
       <c r="D275" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E275" s="9" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="276" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A276" s="3"/>
       <c r="B276" s="24"/>
       <c r="C276" s="20" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="D276" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E276" s="9" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="277" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A277" s="3"/>
       <c r="B277" s="24"/>
       <c r="C277" s="20" t="s">
-        <v>134</v>
+        <v>42</v>
       </c>
       <c r="D277" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E277" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="278" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A278" s="3"/>
       <c r="B278" s="24"/>
       <c r="C278" s="20" t="s">
-        <v>135</v>
+        <v>43</v>
       </c>
       <c r="D278" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E278" s="9" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="279" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A279" s="3"/>
       <c r="B279" s="24"/>
       <c r="C279" s="20" t="s">
-        <v>136</v>
+        <v>44</v>
       </c>
       <c r="D279" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E279" s="9" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="280" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A280" s="3"/>
       <c r="B280" s="24"/>
-      <c r="C280" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="D280" s="65" t="s">
+      <c r="C280" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D280" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E280" s="65" t="s">
-        <v>176</v>
+      <c r="E280" s="9" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="281" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A281" s="3"/>
-      <c r="B281" s="30"/>
-      <c r="C281" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="D281" s="65" t="s">
+      <c r="B281" s="24"/>
+      <c r="C281" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D281" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E281" s="65" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="282" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="E281" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A282" s="3"/>
-      <c r="B282" s="6"/>
-      <c r="C282" s="6"/>
-      <c r="D282" s="6"/>
-      <c r="E282" s="6"/>
-    </row>
-    <row r="283" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B282" s="24"/>
+      <c r="C282" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D282" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E282" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A283" s="3"/>
-      <c r="B283" s="68" t="s">
-        <v>61</v>
-      </c>
-      <c r="C283" s="64" t="s">
-        <v>415</v>
-      </c>
-      <c r="D283" s="54"/>
-      <c r="E283" s="3"/>
+      <c r="B283" s="24"/>
+      <c r="C283" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D283" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E283" s="9" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="284" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A284" s="3"/>
-      <c r="B284" s="3"/>
-      <c r="C284" s="3"/>
-      <c r="D284" s="3"/>
-      <c r="E284" s="3"/>
+      <c r="B284" s="24"/>
+      <c r="C284" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="D284" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E284" s="9" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="285" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A285" s="3"/>
-      <c r="B285" s="20" t="s">
-        <v>210</v>
-      </c>
+      <c r="B285" s="24"/>
       <c r="C285" s="20" t="s">
-        <v>5</v>
+        <v>136</v>
       </c>
       <c r="D285" s="9" t="s">
-        <v>181</v>
+        <v>25</v>
       </c>
       <c r="E285" s="9" t="s">
-        <v>354</v>
+        <v>175</v>
       </c>
     </row>
     <row r="286" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A286" s="3"/>
-      <c r="B286" s="19" t="s">
-        <v>55</v>
-      </c>
+      <c r="B286" s="24"/>
       <c r="C286" s="35" t="s">
-        <v>211</v>
-      </c>
-      <c r="D286" s="67" t="s">
-        <v>180</v>
+        <v>137</v>
+      </c>
+      <c r="D286" s="65" t="s">
+        <v>25</v>
       </c>
       <c r="E286" s="65" t="s">
-        <v>305</v>
+        <v>176</v>
       </c>
     </row>
     <row r="287" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A287" s="3"/>
-      <c r="B287" s="24"/>
-      <c r="C287" s="69" t="s">
-        <v>182</v>
-      </c>
-      <c r="D287" s="58" t="s">
-        <v>180</v>
-      </c>
-      <c r="E287" s="67" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="288" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B287" s="30"/>
+      <c r="C287" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="D287" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="E287" s="65" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A288" s="3"/>
-      <c r="B288" s="11"/>
-      <c r="C288" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D288" s="58" t="s">
-        <v>180</v>
-      </c>
-      <c r="E288" s="9" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="289" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B288" s="6"/>
+      <c r="C288" s="6"/>
+      <c r="D288" s="6"/>
+      <c r="E288" s="6"/>
+    </row>
+    <row r="289" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A289" s="3"/>
-      <c r="B289" s="11"/>
-      <c r="C289" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="D289" s="58" t="s">
-        <v>180</v>
-      </c>
-      <c r="E289" s="9" t="s">
-        <v>474</v>
-      </c>
+      <c r="B289" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="C289" s="64" t="s">
+        <v>415</v>
+      </c>
+      <c r="D289" s="54"/>
+      <c r="E289" s="3"/>
     </row>
     <row r="290" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A290" s="3"/>
-      <c r="B290" s="11"/>
-      <c r="C290" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="D290" s="58" t="s">
-        <v>180</v>
-      </c>
-      <c r="E290" s="9" t="s">
-        <v>416</v>
-      </c>
+      <c r="B290" s="3"/>
+      <c r="C290" s="3"/>
+      <c r="D290" s="3"/>
+      <c r="E290" s="3"/>
     </row>
     <row r="291" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A291" s="3"/>
-      <c r="B291" s="11"/>
-      <c r="C291" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="D291" s="58" t="s">
-        <v>180</v>
+      <c r="B291" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="C291" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D291" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="E291" s="9" t="s">
-        <v>417</v>
+        <v>354</v>
       </c>
     </row>
     <row r="292" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A292" s="3"/>
-      <c r="B292" s="11"/>
-      <c r="C292" s="70" t="s">
-        <v>212</v>
+      <c r="B292" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C292" s="35" t="s">
+        <v>211</v>
       </c>
       <c r="D292" s="67" t="s">
-        <v>213</v>
+        <v>180</v>
       </c>
       <c r="E292" s="65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="293" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A293" s="3"/>
       <c r="B293" s="24"/>
-      <c r="C293" s="70" t="s">
-        <v>195</v>
+      <c r="C293" s="69" t="s">
+        <v>182</v>
       </c>
       <c r="D293" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="E293" s="65" t="s">
-        <v>307</v>
+      <c r="E293" s="67" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="294" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A294" s="3"/>
-      <c r="B294" s="24"/>
-      <c r="C294" s="69" t="s">
-        <v>196</v>
+      <c r="B294" s="11"/>
+      <c r="C294" s="25" t="s">
+        <v>68</v>
       </c>
       <c r="D294" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="E294" s="67" t="s">
-        <v>308</v>
+      <c r="E294" s="9" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="295" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A295" s="3"/>
-      <c r="B295" s="24"/>
-      <c r="C295" s="70" t="s">
-        <v>476</v>
-      </c>
-      <c r="D295" s="67" t="s">
+      <c r="B295" s="11"/>
+      <c r="C295" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="D295" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="E295" s="65" t="s">
-        <v>475</v>
+      <c r="E295" s="9" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="296" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A296" s="3"/>
-      <c r="B296" s="24"/>
-      <c r="C296" s="70" t="s">
-        <v>477</v>
-      </c>
-      <c r="D296" s="67" t="s">
+      <c r="B296" s="11"/>
+      <c r="C296" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="D296" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="E296" s="65" t="s">
-        <v>478</v>
+      <c r="E296" s="9" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="297" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A297" s="3"/>
-      <c r="B297" s="24"/>
-      <c r="C297" s="70" t="s">
-        <v>484</v>
-      </c>
-      <c r="D297" s="67" t="s">
+      <c r="B297" s="11"/>
+      <c r="C297" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="D297" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="E297" s="65" t="s">
-        <v>486</v>
+      <c r="E297" s="9" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="298" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A298" s="3"/>
-      <c r="B298" s="30"/>
+      <c r="B298" s="11"/>
       <c r="C298" s="70" t="s">
-        <v>485</v>
+        <v>212</v>
       </c>
       <c r="D298" s="67" t="s">
+        <v>213</v>
+      </c>
+      <c r="E298" s="65" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A299" s="3"/>
+      <c r="B299" s="24"/>
+      <c r="C299" s="70" t="s">
+        <v>195</v>
+      </c>
+      <c r="D299" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="E298" s="65" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="299" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A299" s="3"/>
-      <c r="B299" s="3"/>
-      <c r="C299" s="3"/>
-      <c r="D299" s="3"/>
-      <c r="E299" s="3"/>
-    </row>
-    <row r="300" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="E299" s="65" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A300" s="3"/>
-      <c r="B300" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C300" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D300" s="3"/>
-      <c r="E300" s="3"/>
+      <c r="B300" s="24"/>
+      <c r="C300" s="69" t="s">
+        <v>196</v>
+      </c>
+      <c r="D300" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="E300" s="67" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="301" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A301" s="3"/>
-      <c r="B301" s="3"/>
-      <c r="C301" s="3"/>
-      <c r="D301" s="3"/>
-      <c r="E301" s="3"/>
+      <c r="B301" s="24"/>
+      <c r="C301" s="70" t="s">
+        <v>476</v>
+      </c>
+      <c r="D301" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="E301" s="65" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="302" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A302" s="3"/>
-      <c r="B302" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="C302" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D302" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="E302" s="9" t="s">
-        <v>48</v>
+      <c r="B302" s="24"/>
+      <c r="C302" s="70" t="s">
+        <v>477</v>
+      </c>
+      <c r="D302" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="E302" s="65" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="303" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A303" s="3"/>
-      <c r="B303" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C303" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="D303" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="E303" s="9" t="s">
-        <v>388</v>
+      <c r="B303" s="24"/>
+      <c r="C303" s="70" t="s">
+        <v>483</v>
+      </c>
+      <c r="D303" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="E303" s="65" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="304" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A304" s="3"/>
-      <c r="B304" s="24"/>
-      <c r="C304" s="35" t="s">
-        <v>214</v>
-      </c>
-      <c r="D304" s="35" t="s">
-        <v>215</v>
+      <c r="B304" s="30"/>
+      <c r="C304" s="70" t="s">
+        <v>484</v>
+      </c>
+      <c r="D304" s="67" t="s">
+        <v>180</v>
       </c>
       <c r="E304" s="65" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="305" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A305" s="3"/>
-      <c r="B305" s="24"/>
-      <c r="C305" s="35" t="s">
-        <v>467</v>
-      </c>
-      <c r="D305" s="35" t="s">
-        <v>468</v>
-      </c>
-      <c r="E305" s="65" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="306" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B305" s="3"/>
+      <c r="C305" s="3"/>
+      <c r="D305" s="3"/>
+      <c r="E305" s="3"/>
+    </row>
+    <row r="306" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A306" s="3"/>
-      <c r="B306" s="24"/>
-      <c r="C306" s="35" t="s">
-        <v>482</v>
-      </c>
-      <c r="D306" s="65" t="s">
-        <v>481</v>
-      </c>
-      <c r="E306" s="65" t="s">
-        <v>483</v>
-      </c>
+      <c r="B306" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C306" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D306" s="3"/>
+      <c r="E306" s="3"/>
     </row>
     <row r="307" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A307" s="3"/>
-      <c r="B307" s="11"/>
-      <c r="C307" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="D307" s="65" t="s">
-        <v>310</v>
-      </c>
-      <c r="E307" s="65" t="s">
-        <v>189</v>
-      </c>
+      <c r="B307" s="3"/>
+      <c r="C307" s="3"/>
+      <c r="D307" s="3"/>
+      <c r="E307" s="3"/>
     </row>
     <row r="308" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A308" s="3"/>
-      <c r="B308" s="11"/>
-      <c r="C308" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="D308" s="65" t="s">
-        <v>311</v>
-      </c>
-      <c r="E308" s="65" t="s">
-        <v>191</v>
+      <c r="B308" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="C308" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D308" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="E308" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="309" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A309" s="3"/>
-      <c r="B309" s="14"/>
-      <c r="C309" s="35" t="s">
+      <c r="B309" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C309" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D309" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="E309" s="9" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A310" s="3"/>
+      <c r="B310" s="24"/>
+      <c r="C310" s="35" t="s">
+        <v>214</v>
+      </c>
+      <c r="D310" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="E310" s="65" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A311" s="3"/>
+      <c r="B311" s="24"/>
+      <c r="C311" s="35" t="s">
+        <v>467</v>
+      </c>
+      <c r="D311" s="35" t="s">
+        <v>468</v>
+      </c>
+      <c r="E311" s="65" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A312" s="3"/>
+      <c r="B312" s="24"/>
+      <c r="C312" s="35" t="s">
+        <v>481</v>
+      </c>
+      <c r="D312" s="65" t="s">
+        <v>480</v>
+      </c>
+      <c r="E312" s="65" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A313" s="3"/>
+      <c r="B313" s="11"/>
+      <c r="C313" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="D313" s="65" t="s">
+        <v>310</v>
+      </c>
+      <c r="E313" s="65" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A314" s="3"/>
+      <c r="B314" s="11"/>
+      <c r="C314" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="D314" s="65" t="s">
+        <v>311</v>
+      </c>
+      <c r="E314" s="65" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A315" s="3"/>
+      <c r="B315" s="14"/>
+      <c r="C315" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="D309" s="65" t="s">
+      <c r="D315" s="65" t="s">
         <v>312</v>
       </c>
-      <c r="E309" s="65" t="s">
+      <c r="E315" s="65" t="s">
         <v>291</v>
       </c>
+    </row>
+    <row r="316" spans="1:5" ht="12.6" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="317" spans="1:5" ht="12.6" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B317" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="C317" s="64" t="s">
+        <v>501</v>
+      </c>
+      <c r="D317" s="54"/>
+      <c r="E317" s="3"/>
+    </row>
+    <row r="318" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B318" s="3"/>
+      <c r="C318" s="3"/>
+      <c r="D318" s="3"/>
+      <c r="E318" s="3"/>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B319" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="C319" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="D319" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="E319" s="9" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B320" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C320" s="20" t="s">
+        <v>502</v>
+      </c>
+      <c r="D320" s="79" t="s">
+        <v>511</v>
+      </c>
+      <c r="E320" s="9" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="321" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B321" s="80"/>
+      <c r="C321" s="20" t="s">
+        <v>505</v>
+      </c>
+      <c r="D321" s="79" t="s">
+        <v>503</v>
+      </c>
+      <c r="E321" s="9" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="322" spans="2:5" ht="12.6" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="323" spans="2:5" ht="12.6" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B323" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="C323" s="64" t="s">
+        <v>507</v>
+      </c>
+      <c r="D323" s="54"/>
+    </row>
+    <row r="325" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B325" s="85" t="s">
+        <v>508</v>
+      </c>
+      <c r="C325" s="86"/>
+      <c r="D325" s="86"/>
+      <c r="E325" s="87"/>
+    </row>
+    <row r="326" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B326" s="85" t="s">
+        <v>513</v>
+      </c>
+      <c r="C326" s="86"/>
+      <c r="D326" s="86"/>
+      <c r="E326" s="87"/>
+    </row>
+    <row r="327" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B327" s="88" t="s">
+        <v>509</v>
+      </c>
+      <c r="C327" s="89"/>
+      <c r="D327" s="89"/>
+      <c r="E327" s="90"/>
+    </row>
+    <row r="328" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B328" s="88" t="s">
+        <v>512</v>
+      </c>
+      <c r="C328" s="89"/>
+      <c r="D328" s="89"/>
+      <c r="E328" s="90"/>
+    </row>
+    <row r="329" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B329" s="91" t="s">
+        <v>510</v>
+      </c>
+      <c r="C329" s="92"/>
+      <c r="D329" s="92"/>
+      <c r="E329" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -8451,8 +8898,8 @@
     <brk id="110" max="16383" man="1"/>
     <brk id="157" max="16383" man="1"/>
     <brk id="213" max="4" man="1"/>
-    <brk id="253" max="4" man="1"/>
-    <brk id="282" max="16383" man="1"/>
+    <brk id="259" max="4" man="1"/>
+    <brk id="288" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>